<commit_message>
updated data and figures for SCWRC poster
</commit_message>
<xml_diff>
--- a/Carbamazepine/Data/Mastersheet_C.xlsx
+++ b/Carbamazepine/Data/Mastersheet_C.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4795f5e3347afba5/Desktop/Dissertation/Lake_Murray/2024-25_Lake_Murray_Bioassays/Carbamazepine/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="123" documentId="8_{FA30851A-7581-4B93-B061-4922F082CD00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B9BAAA6-F730-41EE-BB16-F3CA77D1D551}"/>
+  <xr:revisionPtr revIDLastSave="124" documentId="8_{FA30851A-7581-4B93-B061-4922F082CD00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FA8EF0E-4E75-43AC-BF49-212A29FD9487}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{057AFC9D-ED63-49E6-821F-47BCC2E6B555}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="5" r:id="rId1"/>
-    <sheet name="Biomass" sheetId="6" r:id="rId2"/>
-    <sheet name="Biomass_change" sheetId="7" r:id="rId3"/>
-    <sheet name="Comp" sheetId="3" r:id="rId4"/>
-    <sheet name="FvFm" sheetId="2" r:id="rId5"/>
-    <sheet name="insitu" sheetId="4" r:id="rId6"/>
+    <sheet name="insitu" sheetId="4" r:id="rId2"/>
+    <sheet name="Biomass" sheetId="6" r:id="rId3"/>
+    <sheet name="Biomass_change" sheetId="7" r:id="rId4"/>
+    <sheet name="Comp" sheetId="3" r:id="rId5"/>
+    <sheet name="FvFm" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -859,7 +859,7 @@
   <dimension ref="A1:Q46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43:J43"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2028,6 +2028,62 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CAFA59B-49F2-4CCB-9650-AAFED03CC7D5}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="B2">
+        <v>8.49</v>
+      </c>
+      <c r="C2">
+        <v>9.44</v>
+      </c>
+      <c r="D2">
+        <v>25.75</v>
+      </c>
+      <c r="E2">
+        <v>68.45</v>
+      </c>
+      <c r="F2">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72BB3ABB-AB1E-4BBB-8835-780C5D1899B0}">
   <dimension ref="A1:F46"/>
   <sheetViews>
@@ -2966,7 +3022,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23A8DD69-6E91-4FB7-934F-403B34C7B363}">
   <dimension ref="A1:H46"/>
   <sheetViews>
@@ -4126,7 +4182,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DCD0F97-8D3D-4AF1-89F8-23232854F18D}">
   <dimension ref="A1:F46"/>
   <sheetViews>
@@ -5064,7 +5120,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{891A0728-35A7-476B-A5DD-54943C8C9A75}">
   <dimension ref="A1:F46"/>
   <sheetViews>
@@ -6000,60 +6056,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CAFA59B-49F2-4CCB-9650-AAFED03CC7D5}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>0.39930555555555558</v>
-      </c>
-      <c r="B2">
-        <v>8.49</v>
-      </c>
-      <c r="C2">
-        <v>9.44</v>
-      </c>
-      <c r="D2">
-        <v>25.75</v>
-      </c>
-      <c r="E2">
-        <v>68.45</v>
-      </c>
-      <c r="F2">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>